<commit_message>
Improvements in main, preprocessing, settings file
</commit_message>
<xml_diff>
--- a/settings/settings_Beispiel_GenerateERROR.xlsx
+++ b/settings/settings_Beispiel_GenerateERROR.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Documents\Semesterarbeit FTM\05 - Modell new\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509E3D07-E555-4972-B681-016B1A7ABB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5574F0-35F3-4CF0-81EF-219C01D2180B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{4448D773-169C-4529-85E3-C4726B86DDB4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{4448D773-169C-4529-85E3-C4726B86DDB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="3" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="4" r:id="rId3"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="152">
   <si>
     <t xml:space="preserve">Setting File for MG EV Optimization </t>
   </si>
@@ -476,16 +476,22 @@
     <t>bev_enable_cs</t>
   </si>
   <si>
+    <t>rh_ph</t>
+  </si>
+  <si>
+    <t>rh_ch</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>go</t>
+  </si>
+  <si>
     <t>rh</t>
-  </si>
-  <si>
-    <t>rh_ph</t>
-  </si>
-  <si>
-    <t>rh_ch</t>
-  </si>
-  <si>
-    <t>go</t>
   </si>
 </sst>
 </file>
@@ -913,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67373682-B2FF-4762-AA78-C7C8B3272755}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.45"/>
@@ -972,8 +978,8 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
+      <c r="B6" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -986,8 +992,8 @@
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
+      <c r="B7" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -1029,7 +1035,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -1051,7 +1057,7 @@
     </row>
     <row r="13" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B13" s="2">
         <v>48</v>
@@ -1065,7 +1071,7 @@
     </row>
     <row r="14" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B14" s="2">
         <v>24</v>
@@ -1104,7 +1110,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -1195,8 +1201,8 @@
       <c r="A27" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
+      <c r="B27" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
@@ -1229,8 +1235,8 @@
       <c r="A31" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="2">
-        <v>1</v>
+      <c r="B31" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -1240,8 +1246,8 @@
       <c r="A32" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="2">
-        <v>0</v>
+      <c r="B32" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
@@ -1360,8 +1366,8 @@
       <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
-        <v>1</v>
+      <c r="B42" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
@@ -1371,8 +1377,8 @@
       <c r="A43" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B43" s="2">
-        <v>0</v>
+      <c r="B43" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
@@ -1491,8 +1497,8 @@
       <c r="A53" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="2">
-        <v>1</v>
+      <c r="B53" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C53" t="s">
         <v>3</v>
@@ -1502,8 +1508,8 @@
       <c r="A54" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B54" s="2">
-        <v>0</v>
+      <c r="B54" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C54" t="s">
         <v>3</v>
@@ -1605,8 +1611,8 @@
       <c r="A63" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="2">
-        <v>1</v>
+      <c r="B63" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
@@ -1616,8 +1622,8 @@
       <c r="A64" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="2">
-        <v>0</v>
+      <c r="B64" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
@@ -1806,8 +1812,8 @@
       <c r="A79" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="2">
-        <v>1</v>
+      <c r="B79" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C79" t="s">
         <v>3</v>
@@ -1817,8 +1823,8 @@
       <c r="A80" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B80" s="2">
-        <v>0</v>
+      <c r="B80" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C80" t="s">
         <v>3</v>
@@ -2018,18 +2024,24 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{1758CEB3-2E50-4EDB-A1C0-7F10F46B2D9E}">
       <formula1>"go, rh"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82 B6:B7 B31:B32" xr:uid="{83F9149E-0E25-4669-B401-0B83452863E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82" xr:uid="{83F9149E-0E25-4669-B401-0B83452863E8}">
       <formula1>"False, True, 0, 1"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{02C8EED5-F25F-4186-A02D-EE1AD4AA8937}">
       <formula1>"cbc, gplk, gurobi"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42 B43 B53:B54 B63:B64 B79:B80" xr:uid="{D79CC7DC-A104-47E9-AE23-EC260A36F255}">
-      <formula1>"True, False, 0, 1"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B43 B53:B54 B63:B64 B79:B80" xr:uid="{D79CC7DC-A104-47E9-AE23-EC260A36F255}">
+      <formula1>"True, False,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31 B6 B7" xr:uid="{407269C9-7123-4567-9EAE-D584DF0776AE}">
+      <formula1>"False, True,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27 B32" xr:uid="{E1D29542-326C-4337-96A2-6BE284AD961F}">
+      <formula1>"False, True"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2038,10 +2050,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DCD051-E737-4708-B73F-91479373A432}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6F165B-35C5-4CBE-B7D3-99A444DB276E}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
@@ -2100,8 +2112,8 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
+      <c r="B6" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -2114,8 +2126,8 @@
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
+      <c r="B7" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -2157,7 +2169,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -2179,7 +2191,7 @@
     </row>
     <row r="13" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B13" s="2">
         <v>48</v>
@@ -2193,7 +2205,7 @@
     </row>
     <row r="14" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B14" s="2">
         <v>24</v>
@@ -2323,8 +2335,8 @@
       <c r="A27" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
+      <c r="B27" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
@@ -2357,8 +2369,8 @@
       <c r="A31" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="2">
-        <v>1</v>
+      <c r="B31" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -2368,8 +2380,8 @@
       <c r="A32" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="2">
-        <v>0</v>
+      <c r="B32" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
@@ -2488,8 +2500,8 @@
       <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
-        <v>1</v>
+      <c r="B42" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
@@ -2499,8 +2511,8 @@
       <c r="A43" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B43" s="2">
-        <v>0</v>
+      <c r="B43" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
@@ -2619,8 +2631,8 @@
       <c r="A53" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="2">
-        <v>1</v>
+      <c r="B53" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C53" t="s">
         <v>3</v>
@@ -2630,8 +2642,8 @@
       <c r="A54" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B54" s="2">
-        <v>0</v>
+      <c r="B54" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C54" t="s">
         <v>3</v>
@@ -2733,8 +2745,8 @@
       <c r="A63" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="2">
-        <v>1</v>
+      <c r="B63" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
@@ -2744,8 +2756,8 @@
       <c r="A64" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="2">
-        <v>0</v>
+      <c r="B64" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
@@ -2934,8 +2946,8 @@
       <c r="A79" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="2">
-        <v>1</v>
+      <c r="B79" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C79" t="s">
         <v>3</v>
@@ -2945,8 +2957,8 @@
       <c r="A80" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B80" s="2">
-        <v>0</v>
+      <c r="B80" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C80" t="s">
         <v>3</v>
@@ -3146,17 +3158,23 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B43 B53:B54 B63:B64 B79:B80" xr:uid="{24B0B891-00EA-486A-99CC-E8485D96626D}">
-      <formula1>"True, False, 0, 1"</formula1>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27 B32" xr:uid="{60A8338A-A167-4793-BB50-F6A9B6C817DF}">
+      <formula1>"False, True"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{4B0B194A-E967-41D7-AC88-3E0A13435B13}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31 B6:B7" xr:uid="{5FCBE75C-8735-41FE-B214-89561977391A}">
+      <formula1>"False, True,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B43 B53:B54 B63:B64 B79:B80" xr:uid="{BF5D0494-56DD-4EC8-8ABA-1616EAEA60D8}">
+      <formula1>"True, False,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{0DE4D40B-B6F8-4C98-9293-2CFAC45DE462}">
       <formula1>"cbc, gplk, gurobi"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82 B6:B7 B31:B32" xr:uid="{35F3A501-0666-421F-B54B-663E5E6AD64E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82" xr:uid="{03B2F029-4A8F-40A5-A301-7F6B0DD7761D}">
       <formula1>"False, True, 0, 1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{5E11580E-2589-4930-98C6-E274C01DB0DE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{44445503-4D29-4401-BCD7-B9B8A8B8F6F9}">
       <formula1>"go, rh"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3166,11 +3184,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9985042-84AC-4ABA-B4DA-3D7AAD87EE7D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2054ED9D-66EC-4FB8-B3DE-5C227B8FF4E3}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.45"/>
@@ -3228,8 +3246,8 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
+      <c r="B6" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -3242,8 +3260,8 @@
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
+      <c r="B7" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -3285,7 +3303,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -3307,7 +3325,7 @@
     </row>
     <row r="13" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B13" s="2">
         <v>48</v>
@@ -3321,7 +3339,7 @@
     </row>
     <row r="14" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B14" s="2">
         <v>24</v>
@@ -3360,7 +3378,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -3451,8 +3469,8 @@
       <c r="A27" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
+      <c r="B27" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
@@ -3485,8 +3503,8 @@
       <c r="A31" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="2">
-        <v>1</v>
+      <c r="B31" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -3496,8 +3514,8 @@
       <c r="A32" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="2">
-        <v>0</v>
+      <c r="B32" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
@@ -3616,8 +3634,8 @@
       <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
-        <v>1</v>
+      <c r="B42" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
@@ -3627,8 +3645,8 @@
       <c r="A43" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B43" s="2">
-        <v>0</v>
+      <c r="B43" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
@@ -3747,8 +3765,8 @@
       <c r="A53" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="2">
-        <v>1</v>
+      <c r="B53" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C53" t="s">
         <v>3</v>
@@ -3758,8 +3776,8 @@
       <c r="A54" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B54" s="2">
-        <v>0</v>
+      <c r="B54" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C54" t="s">
         <v>3</v>
@@ -3861,8 +3879,8 @@
       <c r="A63" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="2">
-        <v>1</v>
+      <c r="B63" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
@@ -3872,8 +3890,8 @@
       <c r="A64" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="2">
-        <v>0</v>
+      <c r="B64" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
@@ -4062,8 +4080,8 @@
       <c r="A79" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="2">
-        <v>1</v>
+      <c r="B79" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C79" t="s">
         <v>3</v>
@@ -4073,8 +4091,8 @@
       <c r="A80" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B80" s="2">
-        <v>0</v>
+      <c r="B80" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C80" t="s">
         <v>3</v>
@@ -4274,17 +4292,23 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B43 B53:B54 B63:B64 B79:B80" xr:uid="{6CF93D16-0BC0-485A-B2C3-828EEA80D267}">
-      <formula1>"True, False, 0, 1"</formula1>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27 B32" xr:uid="{140A24D9-2601-4B65-A0E6-75C114FDB237}">
+      <formula1>"False, True"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{C6F9116A-4AC9-4AA9-A3AA-A8D56A7C34F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31 B6:B7" xr:uid="{D0576486-56DE-4BBA-855F-83D95E5A81C6}">
+      <formula1>"False, True,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B43 B53:B54 B63:B64 B79:B80" xr:uid="{F2959E06-33EA-4C7E-869E-CF5B7237D207}">
+      <formula1>"True, False,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{8F166491-3624-4A05-B6C0-C0A116F68BBB}">
       <formula1>"cbc, gplk, gurobi"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82 B6:B7 B31:B32" xr:uid="{E4FD54A6-0A89-4009-9374-43CEAC7E688D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82" xr:uid="{D7D9A4FB-56B1-48E2-A0EB-C04B17908801}">
       <formula1>"False, True, 0, 1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{572572E0-F90C-4A58-AECE-E49B2E4B219C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{E374C02C-5D75-43CF-BAD3-1B66B6EAA288}">
       <formula1>"go, rh"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>